<commit_message>
feat: Add xlwings-based Excel file generators for proper integration testing
- Create xlwings generators for 4 Excel files added this week
- xlwings_information.py: INFORMATION.xlsx with IS* function tests
- xlwings_logical.py: logical.xlsx with AND, OR, TRUE, FALSE tests
- xlwings_math.py: MATH.xlsx with FLOOR, TRUNC, SIGN, LOG tests
- xlwings_text.py: TEXT.xlsx with LEFT, UPPER, LOWER, TRIM tests
- generate_all_xlwings.py: Master script to run all generators
- README_XLWINGS.md: Complete usage documentation

These generators use xlwings to create Excel files with real Excel
calculations, ensuring integration tests compare xlcalculator against
Excel's actual behavior rather than manual calculations.

Requires Windows with Excel for generation. Generated files will contain
both formulas and Excel's calculated values for proper compatibility testing.

Co-authored-by: Ona <no-reply@ona.com>
</commit_message>
<xml_diff>
--- a/tests/resources/INFORMATION.xlsx
+++ b/tests/resources/INFORMATION.xlsx
@@ -425,33 +425,26 @@
       <c r="A1" t="n">
         <v>123</v>
       </c>
-      <c r="B1">
-        <f>ISNUMBER(A1)</f>
-        <v/>
-      </c>
-      <c r="C1">
-        <f>ISTEXT(A1)</f>
-        <v/>
-      </c>
-      <c r="D1">
-        <f>ISBLANK(A1)</f>
-        <v/>
-      </c>
-      <c r="E1">
-        <f>ISERROR(A1)</f>
-        <v/>
-      </c>
-      <c r="F1">
-        <f>ISNA(A1)</f>
-        <v/>
-      </c>
-      <c r="G1">
-        <f>ISERR(A1)</f>
-        <v/>
-      </c>
-      <c r="J1">
-        <f>NA()</f>
-        <v/>
+      <c r="B1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J1" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2">
@@ -460,44 +453,36 @@
           <t>Hello</t>
         </is>
       </c>
-      <c r="B2">
-        <f>ISNUMBER(A2)</f>
-        <v/>
-      </c>
-      <c r="C2">
-        <f>ISTEXT(A2)</f>
-        <v/>
-      </c>
-      <c r="D2">
-        <f>ISBLANK(A2)</f>
-        <v/>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="b">
         <v>1</v>
       </c>
-      <c r="B3">
-        <f>ISNUMBER(A3)</f>
-        <v/>
-      </c>
-      <c r="C3">
-        <f>ISTEXT(A3)</f>
-        <v/>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4">
-        <f>ISNUMBER(A4)</f>
-        <v/>
-      </c>
-      <c r="C4">
-        <f>ISTEXT(A4)</f>
-        <v/>
-      </c>
-      <c r="D4">
-        <f>ISBLANK(A4)</f>
-        <v/>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -505,29 +490,23 @@
         <f>1/0</f>
         <v/>
       </c>
-      <c r="B5">
-        <f>ISNUMBER(123)</f>
-        <v/>
-      </c>
-      <c r="C5">
-        <f>ISTEXT("test")</f>
-        <v/>
-      </c>
-      <c r="D5">
-        <f>ISBLANK("")</f>
-        <v/>
-      </c>
-      <c r="E5">
-        <f>ISERROR(A5)</f>
-        <v/>
-      </c>
-      <c r="F5">
-        <f>ISNA(A5)</f>
-        <v/>
-      </c>
-      <c r="G5">
-        <f>ISERR(A5)</f>
-        <v/>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -535,73 +514,61 @@
         <f>NA()</f>
         <v/>
       </c>
-      <c r="E6">
-        <f>ISERROR(A6)</f>
-        <v/>
-      </c>
-      <c r="F6">
-        <f>ISNA(A6)</f>
-        <v/>
-      </c>
-      <c r="G6">
-        <f>ISERR(A6)</f>
-        <v/>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>4</v>
       </c>
-      <c r="E7">
-        <f>ISERROR(1/0)</f>
-        <v/>
-      </c>
-      <c r="H7">
-        <f>ISEVEN(A7)</f>
-        <v/>
-      </c>
-      <c r="I7">
-        <f>ISODD(A7)</f>
-        <v/>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>5</v>
       </c>
-      <c r="H8">
-        <f>ISEVEN(A8)</f>
-        <v/>
-      </c>
-      <c r="I8">
-        <f>ISODD(A8)</f>
-        <v/>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>0</v>
       </c>
-      <c r="H9">
-        <f>ISEVEN(A9)</f>
-        <v/>
-      </c>
-      <c r="I9">
-        <f>ISODD(A9)</f>
-        <v/>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>-3</v>
       </c>
-      <c r="H10">
-        <f>ISEVEN(A10)</f>
-        <v/>
-      </c>
-      <c r="I10">
-        <f>ISODD(A10)</f>
-        <v/>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>